<commit_message>
Subo el integrador y cosas
</commit_message>
<xml_diff>
--- a/Actividades/Femp03011/Flujo_de_fondos (1).xlsx
+++ b/Actividades/Femp03011/Flujo_de_fondos (1).xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leonardo\Desktop\Leonardo\proyectofinal2019\Actividades\Femp03011\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AB2597B-1F7C-43F7-A9A5-2A6BC944B964}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F2525C9-48FF-40C8-9828-AFA9A1D0EEE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Formula" sheetId="1" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="201">
   <si>
     <r>
       <t xml:space="preserve">Flujo de fondos </t>
@@ -837,35 +837,6 @@
     </r>
     <r>
       <rPr>
-        <b/>
-        <sz val="26"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">- 8231331767 (No rentable) </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">TRR= </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="26"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">- 8231331767 (No rentable) </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">TRR= </t>
-    </r>
-    <r>
-      <rPr>
         <sz val="22"/>
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
@@ -873,6 +844,10 @@
       </rPr>
       <t xml:space="preserve">- 8,231331767 (No rentable) </t>
     </r>
+  </si>
+  <si>
+    <t>OBSERVACIÓN: Los costes relacionados con las unidades de apoyo de secretaria y unidades de linea como gerencia general y las gerencias dependientes de la misma, 
+no han sido tomadas en cuenta por razones de tiempo asi como tambien se hace el supuesto simplificador de que las mismas son terciarizadas</t>
   </si>
 </sst>
 </file>
@@ -2761,7 +2736,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="252">
+  <cellXfs count="254">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2999,6 +2974,10 @@
     <xf numFmtId="170" fontId="23" fillId="5" borderId="129" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="166" fontId="12" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3038,10 +3017,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -3076,14 +3051,6 @@
     <xf numFmtId="170" fontId="12" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="88" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3095,6 +3062,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="109" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="88" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3115,6 +3094,32 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="93" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="80" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3124,44 +3129,20 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="81" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="93" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="80" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="111" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="111" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="111" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="118" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="118" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="111" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3550,10 +3531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1000"/>
+  <dimension ref="A1:AH1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -3572,50 +3553,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="182.25" customHeight="1">
-      <c r="A1" s="178" t="s">
+      <c r="A1" s="180" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="179"/>
-      <c r="C1" s="179"/>
-      <c r="D1" s="179"/>
-      <c r="E1" s="179"/>
-      <c r="F1" s="179"/>
-      <c r="G1" s="179"/>
-      <c r="H1" s="179"/>
-      <c r="I1" s="180"/>
+      <c r="B1" s="181"/>
+      <c r="C1" s="181"/>
+      <c r="D1" s="181"/>
+      <c r="E1" s="181"/>
+      <c r="F1" s="181"/>
+      <c r="G1" s="181"/>
+      <c r="H1" s="181"/>
+      <c r="I1" s="182"/>
       <c r="J1" s="29"/>
     </row>
     <row r="2" spans="1:10" ht="25.5" customHeight="1">
-      <c r="A2" s="181"/>
-      <c r="B2" s="182"/>
-      <c r="C2" s="182"/>
-      <c r="D2" s="182"/>
-      <c r="E2" s="182"/>
-      <c r="F2" s="182"/>
-      <c r="G2" s="182"/>
-      <c r="H2" s="182"/>
-      <c r="I2" s="183"/>
+      <c r="A2" s="183"/>
+      <c r="B2" s="184"/>
+      <c r="C2" s="184"/>
+      <c r="D2" s="184"/>
+      <c r="E2" s="184"/>
+      <c r="F2" s="184"/>
+      <c r="G2" s="184"/>
+      <c r="H2" s="184"/>
+      <c r="I2" s="185"/>
       <c r="J2" s="29"/>
     </row>
     <row r="3" spans="1:10" ht="39" customHeight="1">
-      <c r="A3" s="184" t="s">
+      <c r="A3" s="186" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="185"/>
-      <c r="C3" s="175" t="s">
+      <c r="B3" s="187"/>
+      <c r="C3" s="177" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="176"/>
-      <c r="E3" s="176"/>
-      <c r="F3" s="176"/>
-      <c r="G3" s="176"/>
-      <c r="H3" s="176"/>
-      <c r="I3" s="177"/>
+      <c r="D3" s="178"/>
+      <c r="E3" s="178"/>
+      <c r="F3" s="178"/>
+      <c r="G3" s="178"/>
+      <c r="H3" s="178"/>
+      <c r="I3" s="179"/>
       <c r="J3" s="29"/>
     </row>
     <row r="4" spans="1:10" ht="47.25" hidden="1" customHeight="1">
-      <c r="A4" s="186"/>
-      <c r="B4" s="187"/>
+      <c r="A4" s="188"/>
+      <c r="B4" s="189"/>
       <c r="C4" s="30"/>
       <c r="D4" s="31"/>
       <c r="E4" s="32"/>
@@ -3625,12 +3606,12 @@
       <c r="I4" s="32"/>
     </row>
     <row r="5" spans="1:10" ht="42" customHeight="1">
-      <c r="A5" s="181"/>
-      <c r="B5" s="188"/>
-      <c r="C5" s="189" t="s">
+      <c r="A5" s="183"/>
+      <c r="B5" s="190"/>
+      <c r="C5" s="191" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="190"/>
+      <c r="D5" s="192"/>
       <c r="E5" s="34" t="s">
         <v>12</v>
       </c>
@@ -3649,14 +3630,14 @@
       <c r="J5" s="36"/>
     </row>
     <row r="6" spans="1:10" ht="30">
-      <c r="A6" s="193" t="s">
+      <c r="A6" s="195" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="174"/>
-      <c r="C6" s="191" t="s">
+      <c r="B6" s="176"/>
+      <c r="C6" s="193" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="192"/>
+      <c r="D6" s="194"/>
       <c r="E6" s="37">
         <f>'Tablas Calculadas '!I8 *0.8</f>
         <v>10698041.867946668</v>
@@ -3682,14 +3663,14 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="30">
-      <c r="A7" s="173" t="s">
+      <c r="A7" s="175" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="174"/>
-      <c r="C7" s="171" t="s">
+      <c r="B7" s="176"/>
+      <c r="C7" s="173" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="172"/>
+      <c r="D7" s="174"/>
       <c r="E7" s="40">
         <f>'Tablas Calculadas '!C61*-1</f>
         <v>-11809488</v>
@@ -3712,14 +3693,14 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="30">
-      <c r="A8" s="173" t="s">
+      <c r="A8" s="175" t="s">
         <v>58</v>
       </c>
-      <c r="B8" s="174"/>
-      <c r="C8" s="171" t="s">
+      <c r="B8" s="176"/>
+      <c r="C8" s="173" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="172"/>
+      <c r="D8" s="174"/>
       <c r="E8" s="40">
         <f>'Tablas Calculadas '!B61*-1</f>
         <v>-584877.11999999988</v>
@@ -3743,10 +3724,10 @@
       <c r="J8" s="29"/>
     </row>
     <row r="9" spans="1:10" ht="30">
-      <c r="A9" s="194" t="s">
+      <c r="A9" s="215" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="195"/>
+      <c r="B9" s="216"/>
       <c r="C9" s="200" t="s">
         <v>25</v>
       </c>
@@ -3774,14 +3755,14 @@
       <c r="J9" s="29"/>
     </row>
     <row r="10" spans="1:10" ht="30">
-      <c r="A10" s="212" t="s">
+      <c r="A10" s="219" t="s">
         <v>84</v>
       </c>
-      <c r="B10" s="213"/>
+      <c r="B10" s="220"/>
       <c r="C10" s="202" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="192"/>
+      <c r="D10" s="194"/>
       <c r="E10" s="37">
         <f t="shared" ref="E10:I10" si="0">SUM(E6:E9)</f>
         <v>-2235009.9720533323</v>
@@ -3804,10 +3785,10 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="30">
-      <c r="A11" s="194" t="s">
+      <c r="A11" s="215" t="s">
         <v>86</v>
       </c>
-      <c r="B11" s="195"/>
+      <c r="B11" s="216"/>
       <c r="C11" s="203" t="s">
         <v>25</v>
       </c>
@@ -3835,14 +3816,14 @@
       <c r="J11" s="29"/>
     </row>
     <row r="12" spans="1:10" ht="30">
-      <c r="A12" s="212" t="s">
+      <c r="A12" s="219" t="s">
         <v>88</v>
       </c>
-      <c r="B12" s="213"/>
+      <c r="B12" s="220"/>
       <c r="C12" s="204" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="192"/>
+      <c r="D12" s="194"/>
       <c r="E12" s="37">
         <f t="shared" ref="E12:I12" si="2">E10-E11</f>
         <v>-2235009.9720533323</v>
@@ -3866,12 +3847,12 @@
       <c r="J12" s="29"/>
     </row>
     <row r="13" spans="1:10" ht="30">
-      <c r="A13" s="173" t="s">
+      <c r="A13" s="175" t="s">
         <v>98</v>
       </c>
-      <c r="B13" s="174"/>
+      <c r="B13" s="176"/>
       <c r="C13" s="205"/>
-      <c r="D13" s="172"/>
+      <c r="D13" s="174"/>
       <c r="E13" s="126">
         <f>-E8</f>
         <v>584877.11999999988</v>
@@ -3895,14 +3876,14 @@
       <c r="J13" s="29"/>
     </row>
     <row r="14" spans="1:10" ht="30">
-      <c r="A14" s="217" t="s">
+      <c r="A14" s="213" t="s">
         <v>138</v>
       </c>
-      <c r="B14" s="218"/>
+      <c r="B14" s="214"/>
       <c r="C14" s="209">
         <v>-890454.4</v>
       </c>
-      <c r="D14" s="172"/>
+      <c r="D14" s="174"/>
       <c r="E14" s="136" t="s">
         <v>25</v>
       </c>
@@ -3921,10 +3902,10 @@
       <c r="J14" s="29"/>
     </row>
     <row r="15" spans="1:10" ht="30">
-      <c r="A15" s="194" t="s">
+      <c r="A15" s="215" t="s">
         <v>160</v>
       </c>
-      <c r="B15" s="195"/>
+      <c r="B15" s="216"/>
       <c r="C15" s="206"/>
       <c r="D15" s="201"/>
       <c r="E15" s="158"/>
@@ -3938,10 +3919,10 @@
       <c r="J15" s="29"/>
     </row>
     <row r="16" spans="1:10" ht="30">
-      <c r="A16" s="210" t="s">
+      <c r="A16" s="217" t="s">
         <v>196</v>
       </c>
-      <c r="B16" s="211"/>
+      <c r="B16" s="218"/>
       <c r="C16" s="207">
         <f>C14</f>
         <v>-890454.4</v>
@@ -3969,11 +3950,11 @@
       </c>
       <c r="J16" s="29"/>
     </row>
-    <row r="17" spans="1:10" ht="30">
-      <c r="A17" s="214" t="s">
+    <row r="17" spans="1:34" ht="30">
+      <c r="A17" s="210" t="s">
         <v>197</v>
       </c>
-      <c r="B17" s="215"/>
+      <c r="B17" s="211"/>
       <c r="C17" s="196">
         <v>1</v>
       </c>
@@ -3995,8 +3976,8 @@
       </c>
       <c r="J17" s="29"/>
     </row>
-    <row r="18" spans="1:10" ht="33.75">
-      <c r="A18" s="216" t="s">
+    <row r="18" spans="1:34" ht="33.75">
+      <c r="A18" s="212" t="s">
         <v>198</v>
       </c>
       <c r="B18" s="199"/>
@@ -4026,71 +4007,133 @@
         <v>11012257.341155654</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:34">
       <c r="A19" s="33"/>
       <c r="B19" s="33"/>
       <c r="C19" s="33"/>
     </row>
-    <row r="20" spans="1:10" ht="15" customHeight="1">
+    <row r="20" spans="1:34" ht="15" customHeight="1">
       <c r="B20" s="33"/>
     </row>
-    <row r="21" spans="1:10" ht="28.5">
-      <c r="A21" s="251" t="s">
-        <v>201</v>
+    <row r="21" spans="1:34" ht="28.5">
+      <c r="A21" s="171" t="s">
+        <v>199</v>
       </c>
       <c r="B21" s="33"/>
       <c r="C21" s="33"/>
       <c r="D21" s="33"/>
     </row>
-    <row r="22" spans="1:10" ht="15.75" customHeight="1">
+    <row r="22" spans="1:34" ht="15.75" customHeight="1">
       <c r="A22" s="169"/>
       <c r="B22" s="33"/>
       <c r="C22" s="33"/>
       <c r="D22" s="33"/>
       <c r="F22" s="170"/>
     </row>
-    <row r="23" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A23" s="169"/>
-      <c r="B23" s="33"/>
-      <c r="C23" s="33"/>
-      <c r="D23" s="33"/>
-      <c r="F23" s="170"/>
-    </row>
-    <row r="24" spans="1:10" ht="15.75" customHeight="1">
-      <c r="B24" s="33"/>
-      <c r="C24" s="33"/>
-      <c r="D24" s="33"/>
-    </row>
-    <row r="25" spans="1:10" ht="15.75" customHeight="1">
+    <row r="23" spans="1:34" ht="79.5" customHeight="1">
+      <c r="A23" s="253" t="s">
+        <v>200</v>
+      </c>
+      <c r="B23" s="253"/>
+      <c r="C23" s="253"/>
+      <c r="D23" s="253"/>
+      <c r="E23" s="253"/>
+      <c r="F23" s="253"/>
+      <c r="G23" s="253"/>
+      <c r="H23" s="253"/>
+      <c r="I23" s="253"/>
+      <c r="J23" s="172"/>
+      <c r="K23" s="172"/>
+      <c r="L23" s="172"/>
+      <c r="M23" s="172"/>
+      <c r="N23" s="172"/>
+      <c r="O23" s="172"/>
+      <c r="P23" s="172"/>
+      <c r="Q23" s="172"/>
+      <c r="R23" s="172"/>
+      <c r="S23" s="172"/>
+      <c r="T23" s="172"/>
+      <c r="U23" s="172"/>
+      <c r="V23" s="172"/>
+      <c r="W23" s="172"/>
+      <c r="X23" s="172"/>
+      <c r="Y23" s="172"/>
+      <c r="Z23" s="172"/>
+      <c r="AA23" s="172"/>
+      <c r="AB23" s="172"/>
+      <c r="AC23" s="172"/>
+      <c r="AD23" s="172"/>
+      <c r="AE23" s="172"/>
+      <c r="AF23" s="172"/>
+      <c r="AG23" s="172"/>
+      <c r="AH23" s="172"/>
+    </row>
+    <row r="24" spans="1:34" ht="15.75" customHeight="1">
+      <c r="A24" s="172"/>
+      <c r="B24" s="172"/>
+      <c r="C24" s="172"/>
+      <c r="D24" s="172"/>
+      <c r="E24" s="172"/>
+      <c r="F24" s="172"/>
+      <c r="G24" s="172"/>
+      <c r="H24" s="172"/>
+      <c r="I24" s="172"/>
+      <c r="J24" s="172"/>
+      <c r="K24" s="172"/>
+      <c r="L24" s="172"/>
+      <c r="M24" s="172"/>
+      <c r="N24" s="172"/>
+      <c r="O24" s="172"/>
+      <c r="P24" s="172"/>
+      <c r="Q24" s="172"/>
+      <c r="R24" s="172"/>
+      <c r="S24" s="172"/>
+      <c r="T24" s="172"/>
+      <c r="U24" s="172"/>
+      <c r="V24" s="172"/>
+      <c r="W24" s="172"/>
+      <c r="X24" s="172"/>
+      <c r="Y24" s="172"/>
+      <c r="Z24" s="172"/>
+      <c r="AA24" s="172"/>
+      <c r="AB24" s="172"/>
+      <c r="AC24" s="172"/>
+      <c r="AD24" s="172"/>
+      <c r="AE24" s="172"/>
+      <c r="AF24" s="172"/>
+      <c r="AG24" s="172"/>
+      <c r="AH24" s="172"/>
+    </row>
+    <row r="25" spans="1:34" ht="15.75" customHeight="1">
       <c r="B25" s="33"/>
       <c r="C25" s="33"/>
       <c r="D25" s="33"/>
     </row>
-    <row r="26" spans="1:10" ht="15.75" customHeight="1">
+    <row r="26" spans="1:34" ht="15.75" customHeight="1">
       <c r="B26" s="33"/>
       <c r="C26" s="33"/>
       <c r="D26" s="33"/>
     </row>
-    <row r="27" spans="1:10" ht="15.75" customHeight="1">
+    <row r="27" spans="1:34" ht="15.75" customHeight="1">
       <c r="B27" s="33"/>
       <c r="C27" s="33"/>
       <c r="D27" s="33"/>
     </row>
-    <row r="28" spans="1:10" ht="15.75" customHeight="1">
+    <row r="28" spans="1:34" ht="15.75" customHeight="1">
       <c r="B28" s="33"/>
       <c r="D28" s="33"/>
     </row>
-    <row r="29" spans="1:10" ht="15.75" customHeight="1">
+    <row r="29" spans="1:34" ht="15.75" customHeight="1">
       <c r="B29" s="33"/>
       <c r="D29" s="33"/>
     </row>
-    <row r="30" spans="1:10" ht="15.75" customHeight="1">
+    <row r="30" spans="1:34" ht="15.75" customHeight="1">
       <c r="B30" s="33"/>
     </row>
-    <row r="31" spans="1:10" ht="15.75" customHeight="1">
+    <row r="31" spans="1:34" ht="15.75" customHeight="1">
       <c r="B31" s="33"/>
     </row>
-    <row r="32" spans="1:10" ht="15.75" customHeight="1">
+    <row r="32" spans="1:34" ht="15.75" customHeight="1">
       <c r="B32" s="33"/>
     </row>
     <row r="33" spans="2:2" ht="15.75" customHeight="1">
@@ -6998,27 +7041,23 @@
       <c r="B1000" s="33"/>
     </row>
   </sheetData>
-  <mergeCells count="30">
+  <mergeCells count="31">
+    <mergeCell ref="A23:I23"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C14:D14"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="C3:I3"/>
@@ -7029,6 +7068,11 @@
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
   </mergeCells>
   <conditionalFormatting sqref="C14:I14 C16:I18 C15 E6:I15">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
@@ -7069,18 +7113,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="205.5" customHeight="1">
-      <c r="A1" s="219" t="s">
+      <c r="A1" s="221" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="220"/>
-      <c r="C1" s="220"/>
-      <c r="D1" s="220"/>
-      <c r="E1" s="220"/>
-      <c r="F1" s="220"/>
-      <c r="G1" s="220"/>
-      <c r="H1" s="220"/>
-      <c r="I1" s="220"/>
-      <c r="J1" s="220"/>
+      <c r="B1" s="222"/>
+      <c r="C1" s="222"/>
+      <c r="D1" s="222"/>
+      <c r="E1" s="222"/>
+      <c r="F1" s="222"/>
+      <c r="G1" s="222"/>
+      <c r="H1" s="222"/>
+      <c r="I1" s="222"/>
+      <c r="J1" s="222"/>
     </row>
     <row r="2" spans="1:10" ht="14.25">
       <c r="A2" s="1"/>
@@ -7158,7 +7202,7 @@
       <c r="I6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J6" s="225" t="s">
+      <c r="J6" s="227" t="s">
         <v>10</v>
       </c>
     </row>
@@ -7177,7 +7221,7 @@
         <f>B7*'Tablas Calculadas '!E20+C7*'Tablas Calculadas '!E21+F7*'Tablas Calculadas '!E39+G7*'Tablas Calculadas '!E40+'Tablas Calculadas '!E41*H7+D7*'Tablas Calculadas '!E27+E7*'Tablas Calculadas '!E33</f>
         <v>0</v>
       </c>
-      <c r="J7" s="226"/>
+      <c r="J7" s="228"/>
     </row>
     <row r="8" spans="1:10" ht="14.25">
       <c r="A8" s="10" t="s">
@@ -7202,7 +7246,7 @@
         <f>B8*'Tablas Calculadas '!E20+C8*'Tablas Calculadas '!E22+F8*'Tablas Calculadas '!E42+G8*'Tablas Calculadas '!E43+'Tablas Calculadas '!E44*H8+D8*'Tablas Calculadas '!E28+E8*'Tablas Calculadas '!E34</f>
         <v>13372552.334933333</v>
       </c>
-      <c r="J8" s="226"/>
+      <c r="J8" s="228"/>
     </row>
     <row r="9" spans="1:10" ht="14.25">
       <c r="A9" s="10" t="s">
@@ -7225,7 +7269,7 @@
         <f>B9*'Tablas Calculadas '!E20+C9*'Tablas Calculadas '!E23+F9*'Tablas Calculadas '!E45+G9*'Tablas Calculadas '!E46+H9*'Tablas Calculadas '!E47+D9*'Tablas Calculadas '!E29+E9*'Tablas Calculadas '!E35</f>
         <v>3057963.2529333332</v>
       </c>
-      <c r="J9" s="226"/>
+      <c r="J9" s="228"/>
     </row>
     <row r="10" spans="1:10" ht="15" customHeight="1">
       <c r="A10" s="10" t="s">
@@ -7248,7 +7292,7 @@
         <f>B10*'Tablas Calculadas '!E20+C10*'Tablas Calculadas '!E24+F10*'Tablas Calculadas '!E48+'Tablas Calculadas '!E49*G10+H10*'Tablas Calculadas '!E50+D10*'Tablas Calculadas '!E30+E10*'Tablas Calculadas '!E36</f>
         <v>4532030.391466666</v>
       </c>
-      <c r="J10" s="226"/>
+      <c r="J10" s="228"/>
     </row>
     <row r="11" spans="1:10" ht="15" customHeight="1">
       <c r="A11" s="15" t="s">
@@ -7271,7 +7315,7 @@
         <f>B11*'Tablas Calculadas '!E20+C11*'Tablas Calculadas '!E25+F11*'Tablas Calculadas '!E51+'Tablas Calculadas '!E52*G11+H11*'Tablas Calculadas '!E53+D11*'Tablas Calculadas '!E31+E11*'Tablas Calculadas '!E37</f>
         <v>5526691.8570666667</v>
       </c>
-      <c r="J11" s="226"/>
+      <c r="J11" s="228"/>
     </row>
     <row r="12" spans="1:10" ht="14.25">
       <c r="A12" s="20" t="s">
@@ -7294,7 +7338,7 @@
         <f>B12*'Tablas Calculadas '!E20+C12*'Tablas Calculadas '!E26+F12*'Tablas Calculadas '!E54+'Tablas Calculadas '!E55*G12+H12*'Tablas Calculadas '!E56+D12*'Tablas Calculadas '!E32+E12*'Tablas Calculadas '!E38</f>
         <v>4176815.5392</v>
       </c>
-      <c r="J12" s="226"/>
+      <c r="J12" s="228"/>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="25" t="s">
@@ -7332,7 +7376,7 @@
         <f>SUM(I7:I12)</f>
         <v>30666053.375600003</v>
       </c>
-      <c r="J13" s="227"/>
+      <c r="J13" s="229"/>
     </row>
     <row r="14" spans="1:10" ht="14.25">
       <c r="A14" s="1"/>
@@ -7383,15 +7427,15 @@
       <c r="J17" s="1"/>
     </row>
     <row r="18" spans="1:10" ht="18">
-      <c r="A18" s="221" t="s">
+      <c r="A18" s="223" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="222"/>
-      <c r="C18" s="223" t="s">
+      <c r="B18" s="224"/>
+      <c r="C18" s="225" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="224"/>
-      <c r="E18" s="222"/>
+      <c r="D18" s="226"/>
+      <c r="E18" s="224"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
@@ -8599,10 +8643,10 @@
       <c r="J70" s="1"/>
     </row>
     <row r="71" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A71" s="228" t="s">
+      <c r="A71" s="230" t="s">
         <v>192</v>
       </c>
-      <c r="B71" s="211"/>
+      <c r="B71" s="218"/>
       <c r="C71" s="154" t="s">
         <v>188</v>
       </c>
@@ -9867,17 +9911,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="148.5" customHeight="1">
-      <c r="A1" s="236" t="s">
+      <c r="A1" s="232" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="237"/>
-      <c r="C1" s="237"/>
-      <c r="D1" s="237"/>
-      <c r="E1" s="237"/>
-      <c r="F1" s="237"/>
-      <c r="G1" s="237"/>
-      <c r="H1" s="237"/>
-      <c r="I1" s="211"/>
+      <c r="B1" s="233"/>
+      <c r="C1" s="233"/>
+      <c r="D1" s="233"/>
+      <c r="E1" s="233"/>
+      <c r="F1" s="233"/>
+      <c r="G1" s="233"/>
+      <c r="H1" s="233"/>
+      <c r="I1" s="218"/>
     </row>
     <row r="2" spans="1:9" ht="14.25">
       <c r="H2" s="1"/>
@@ -9904,10 +9948,10 @@
     <row r="6" spans="1:9" ht="18">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
-      <c r="C6" s="228" t="s">
+      <c r="C6" s="230" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="211"/>
+      <c r="D6" s="218"/>
       <c r="E6" s="41">
         <v>1</v>
       </c>
@@ -9918,10 +9962,10 @@
       <c r="I6" s="1"/>
     </row>
     <row r="7" spans="1:9" ht="18">
-      <c r="A7" s="228" t="s">
+      <c r="A7" s="230" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="211"/>
+      <c r="B7" s="218"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -9936,7 +9980,7 @@
       <c r="B8" s="43">
         <v>81000</v>
       </c>
-      <c r="C8" s="225" t="s">
+      <c r="C8" s="227" t="s">
         <v>32</v>
       </c>
       <c r="D8" s="44"/>
@@ -9952,7 +9996,7 @@
       <c r="B9" s="45">
         <v>135000</v>
       </c>
-      <c r="C9" s="226"/>
+      <c r="C9" s="228"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -9966,7 +10010,7 @@
       <c r="B10" s="45">
         <v>194000</v>
       </c>
-      <c r="C10" s="234"/>
+      <c r="C10" s="238"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -10098,22 +10142,22 @@
       <c r="I19" s="1"/>
     </row>
     <row r="20" spans="1:9" ht="18">
-      <c r="A20" s="228" t="s">
+      <c r="A20" s="230" t="s">
         <v>43</v>
       </c>
-      <c r="B20" s="237"/>
-      <c r="C20" s="237"/>
-      <c r="D20" s="211"/>
+      <c r="B20" s="233"/>
+      <c r="C20" s="233"/>
+      <c r="D20" s="218"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
     <row r="21" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A21" s="238" t="s">
+      <c r="A21" s="235" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="211"/>
+      <c r="B21" s="218"/>
       <c r="C21" s="47" t="s">
         <v>44</v>
       </c>
@@ -10126,10 +10170,10 @@
       <c r="I21" s="1"/>
     </row>
     <row r="22" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A22" s="239" t="s">
+      <c r="A22" s="236" t="s">
         <v>46</v>
       </c>
-      <c r="B22" s="240"/>
+      <c r="B22" s="237"/>
       <c r="C22" s="55">
         <v>657</v>
       </c>
@@ -10142,10 +10186,10 @@
       <c r="I22" s="1"/>
     </row>
     <row r="23" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A23" s="235" t="s">
+      <c r="A23" s="234" t="s">
         <v>47</v>
       </c>
-      <c r="B23" s="174"/>
+      <c r="B23" s="176"/>
       <c r="C23" s="56">
         <v>200</v>
       </c>
@@ -10158,10 +10202,10 @@
       <c r="I23" s="1"/>
     </row>
     <row r="24" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A24" s="235" t="s">
+      <c r="A24" s="234" t="s">
         <v>48</v>
       </c>
-      <c r="B24" s="174"/>
+      <c r="B24" s="176"/>
       <c r="C24" s="56">
         <v>150</v>
       </c>
@@ -10174,10 +10218,10 @@
       <c r="I24" s="1"/>
     </row>
     <row r="25" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A25" s="245" t="s">
+      <c r="A25" s="231" t="s">
         <v>49</v>
       </c>
-      <c r="B25" s="195"/>
+      <c r="B25" s="216"/>
       <c r="C25" s="59">
         <f>SUM(C22:C24)</f>
         <v>1007</v>
@@ -10199,10 +10243,10 @@
       <c r="I26" s="1"/>
     </row>
     <row r="27" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A27" s="228" t="s">
+      <c r="A27" s="230" t="s">
         <v>55</v>
       </c>
-      <c r="B27" s="211"/>
+      <c r="B27" s="218"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
@@ -10231,7 +10275,7 @@
       <c r="B29" s="63">
         <v>40</v>
       </c>
-      <c r="C29" s="231" t="s">
+      <c r="C29" s="245" t="s">
         <v>59</v>
       </c>
       <c r="D29" s="1"/>
@@ -10247,7 +10291,7 @@
       <c r="B30" s="71">
         <v>46</v>
       </c>
-      <c r="C30" s="232"/>
+      <c r="C30" s="246"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
@@ -10261,7 +10305,7 @@
       <c r="B31" s="71">
         <v>53</v>
       </c>
-      <c r="C31" s="232"/>
+      <c r="C31" s="246"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
@@ -10275,7 +10319,7 @@
       <c r="B32" s="71">
         <v>56</v>
       </c>
-      <c r="C32" s="232"/>
+      <c r="C32" s="246"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
@@ -10289,7 +10333,7 @@
       <c r="B33" s="71">
         <v>64</v>
       </c>
-      <c r="C33" s="232"/>
+      <c r="C33" s="246"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
@@ -10303,7 +10347,7 @@
       <c r="B34" s="74">
         <v>76</v>
       </c>
-      <c r="C34" s="233"/>
+      <c r="C34" s="247"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
@@ -10331,10 +10375,10 @@
       <c r="I36" s="1"/>
     </row>
     <row r="37" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A37" s="228" t="s">
+      <c r="A37" s="230" t="s">
         <v>63</v>
       </c>
-      <c r="B37" s="211"/>
+      <c r="B37" s="218"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
@@ -10379,7 +10423,7 @@
       <c r="B40" s="50">
         <v>8</v>
       </c>
-      <c r="C40" s="229" t="s">
+      <c r="C40" s="243" t="s">
         <v>69</v>
       </c>
       <c r="D40" s="1"/>
@@ -10395,7 +10439,7 @@
       <c r="B41" s="50">
         <v>22</v>
       </c>
-      <c r="C41" s="230"/>
+      <c r="C41" s="244"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
@@ -10643,42 +10687,42 @@
       <c r="I58" s="1"/>
     </row>
     <row r="59" spans="1:13" ht="23.25" customHeight="1">
-      <c r="A59" s="241" t="s">
+      <c r="A59" s="239" t="s">
         <v>94</v>
       </c>
-      <c r="B59" s="215"/>
-      <c r="C59" s="228" t="s">
+      <c r="B59" s="211"/>
+      <c r="C59" s="230" t="s">
         <v>95</v>
       </c>
-      <c r="D59" s="237"/>
-      <c r="E59" s="211"/>
-      <c r="F59" s="244" t="s">
+      <c r="D59" s="233"/>
+      <c r="E59" s="218"/>
+      <c r="F59" s="242" t="s">
         <v>96</v>
       </c>
-      <c r="G59" s="237"/>
-      <c r="H59" s="237"/>
-      <c r="I59" s="237"/>
-      <c r="J59" s="237"/>
-      <c r="K59" s="237"/>
-      <c r="L59" s="237"/>
-      <c r="M59" s="211"/>
+      <c r="G59" s="233"/>
+      <c r="H59" s="233"/>
+      <c r="I59" s="233"/>
+      <c r="J59" s="233"/>
+      <c r="K59" s="233"/>
+      <c r="L59" s="233"/>
+      <c r="M59" s="218"/>
     </row>
     <row r="60" spans="1:13" ht="21" customHeight="1">
-      <c r="A60" s="242"/>
-      <c r="B60" s="243"/>
-      <c r="C60" s="228" t="s">
+      <c r="A60" s="240"/>
+      <c r="B60" s="241"/>
+      <c r="C60" s="230" t="s">
         <v>103</v>
       </c>
-      <c r="D60" s="237"/>
-      <c r="E60" s="237"/>
-      <c r="F60" s="237"/>
-      <c r="G60" s="237"/>
-      <c r="H60" s="237"/>
-      <c r="I60" s="237"/>
-      <c r="J60" s="237"/>
-      <c r="K60" s="237"/>
-      <c r="L60" s="237"/>
-      <c r="M60" s="211"/>
+      <c r="D60" s="233"/>
+      <c r="E60" s="233"/>
+      <c r="F60" s="233"/>
+      <c r="G60" s="233"/>
+      <c r="H60" s="233"/>
+      <c r="I60" s="233"/>
+      <c r="J60" s="233"/>
+      <c r="K60" s="233"/>
+      <c r="L60" s="233"/>
+      <c r="M60" s="218"/>
     </row>
     <row r="61" spans="1:13" ht="15.75" customHeight="1">
       <c r="A61" s="99" t="s">
@@ -12992,19 +13036,19 @@
     <mergeCell ref="C60:M60"/>
     <mergeCell ref="F59:M59"/>
     <mergeCell ref="A27:B27"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="C29:C34"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A25:B25"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="A20:D20"/>
     <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="C29:C34"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C8:C10"/>
     <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A25:B25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -13031,17 +13075,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="117" customHeight="1">
-      <c r="A1" s="236" t="s">
+      <c r="A1" s="232" t="s">
         <v>173</v>
       </c>
-      <c r="B1" s="237"/>
-      <c r="C1" s="237"/>
-      <c r="D1" s="237"/>
-      <c r="E1" s="237"/>
-      <c r="F1" s="237"/>
-      <c r="G1" s="237"/>
-      <c r="H1" s="237"/>
-      <c r="I1" s="211"/>
+      <c r="B1" s="233"/>
+      <c r="C1" s="233"/>
+      <c r="D1" s="233"/>
+      <c r="E1" s="233"/>
+      <c r="F1" s="233"/>
+      <c r="G1" s="233"/>
+      <c r="H1" s="233"/>
+      <c r="I1" s="218"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
@@ -13061,15 +13105,15 @@
       <c r="L2" s="1"/>
     </row>
     <row r="3" spans="1:12" ht="18">
-      <c r="A3" s="228" t="s">
+      <c r="A3" s="230" t="s">
         <v>174</v>
       </c>
-      <c r="B3" s="237"/>
-      <c r="C3" s="237"/>
-      <c r="D3" s="237"/>
-      <c r="E3" s="237"/>
-      <c r="F3" s="237"/>
-      <c r="G3" s="211"/>
+      <c r="B3" s="233"/>
+      <c r="C3" s="233"/>
+      <c r="D3" s="233"/>
+      <c r="E3" s="233"/>
+      <c r="F3" s="233"/>
+      <c r="G3" s="218"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -13080,14 +13124,14 @@
       <c r="A4" s="148" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="246" t="s">
+      <c r="B4" s="248" t="s">
         <v>175</v>
       </c>
-      <c r="C4" s="247"/>
-      <c r="D4" s="247"/>
-      <c r="E4" s="247"/>
-      <c r="F4" s="247"/>
-      <c r="G4" s="174"/>
+      <c r="C4" s="249"/>
+      <c r="D4" s="249"/>
+      <c r="E4" s="249"/>
+      <c r="F4" s="249"/>
+      <c r="G4" s="176"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -13098,14 +13142,14 @@
       <c r="A5" s="148" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="246" t="s">
+      <c r="B5" s="248" t="s">
         <v>176</v>
       </c>
-      <c r="C5" s="247"/>
-      <c r="D5" s="247"/>
-      <c r="E5" s="247"/>
-      <c r="F5" s="247"/>
-      <c r="G5" s="174"/>
+      <c r="C5" s="249"/>
+      <c r="D5" s="249"/>
+      <c r="E5" s="249"/>
+      <c r="F5" s="249"/>
+      <c r="G5" s="176"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -13116,14 +13160,14 @@
       <c r="A6" s="148" t="s">
         <v>177</v>
       </c>
-      <c r="B6" s="246" t="s">
+      <c r="B6" s="248" t="s">
         <v>178</v>
       </c>
-      <c r="C6" s="247"/>
-      <c r="D6" s="247"/>
-      <c r="E6" s="247"/>
-      <c r="F6" s="247"/>
-      <c r="G6" s="174"/>
+      <c r="C6" s="249"/>
+      <c r="D6" s="249"/>
+      <c r="E6" s="249"/>
+      <c r="F6" s="249"/>
+      <c r="G6" s="176"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -13134,14 +13178,14 @@
       <c r="A7" s="148" t="s">
         <v>179</v>
       </c>
-      <c r="B7" s="246" t="s">
+      <c r="B7" s="248" t="s">
         <v>180</v>
       </c>
-      <c r="C7" s="247"/>
-      <c r="D7" s="247"/>
-      <c r="E7" s="247"/>
-      <c r="F7" s="247"/>
-      <c r="G7" s="174"/>
+      <c r="C7" s="249"/>
+      <c r="D7" s="249"/>
+      <c r="E7" s="249"/>
+      <c r="F7" s="249"/>
+      <c r="G7" s="176"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -13152,14 +13196,14 @@
       <c r="A8" s="148" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="246" t="s">
+      <c r="B8" s="248" t="s">
         <v>181</v>
       </c>
-      <c r="C8" s="247"/>
-      <c r="D8" s="247"/>
-      <c r="E8" s="247"/>
-      <c r="F8" s="247"/>
-      <c r="G8" s="174"/>
+      <c r="C8" s="249"/>
+      <c r="D8" s="249"/>
+      <c r="E8" s="249"/>
+      <c r="F8" s="249"/>
+      <c r="G8" s="176"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -13170,14 +13214,14 @@
       <c r="A9" s="148" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="246" t="s">
+      <c r="B9" s="248" t="s">
         <v>182</v>
       </c>
-      <c r="C9" s="247"/>
-      <c r="D9" s="247"/>
-      <c r="E9" s="247"/>
-      <c r="F9" s="247"/>
-      <c r="G9" s="174"/>
+      <c r="C9" s="249"/>
+      <c r="D9" s="249"/>
+      <c r="E9" s="249"/>
+      <c r="F9" s="249"/>
+      <c r="G9" s="176"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -13188,14 +13232,14 @@
       <c r="A10" s="148" t="s">
         <v>183</v>
       </c>
-      <c r="B10" s="248" t="s">
+      <c r="B10" s="252" t="s">
         <v>184</v>
       </c>
-      <c r="C10" s="247"/>
-      <c r="D10" s="247"/>
-      <c r="E10" s="247"/>
-      <c r="F10" s="247"/>
-      <c r="G10" s="174"/>
+      <c r="C10" s="249"/>
+      <c r="D10" s="249"/>
+      <c r="E10" s="249"/>
+      <c r="F10" s="249"/>
+      <c r="G10" s="176"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -13206,14 +13250,14 @@
       <c r="A11" s="148" t="s">
         <v>59</v>
       </c>
-      <c r="B11" s="246" t="s">
+      <c r="B11" s="248" t="s">
         <v>185</v>
       </c>
-      <c r="C11" s="247"/>
-      <c r="D11" s="247"/>
-      <c r="E11" s="247"/>
-      <c r="F11" s="247"/>
-      <c r="G11" s="174"/>
+      <c r="C11" s="249"/>
+      <c r="D11" s="249"/>
+      <c r="E11" s="249"/>
+      <c r="F11" s="249"/>
+      <c r="G11" s="176"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -13224,14 +13268,14 @@
       <c r="A12" s="148" t="s">
         <v>67</v>
       </c>
-      <c r="B12" s="246" t="s">
+      <c r="B12" s="248" t="s">
         <v>186</v>
       </c>
-      <c r="C12" s="247"/>
-      <c r="D12" s="247"/>
-      <c r="E12" s="247"/>
-      <c r="F12" s="247"/>
-      <c r="G12" s="174"/>
+      <c r="C12" s="249"/>
+      <c r="D12" s="249"/>
+      <c r="E12" s="249"/>
+      <c r="F12" s="249"/>
+      <c r="G12" s="176"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -13242,14 +13286,14 @@
       <c r="A13" s="148" t="s">
         <v>69</v>
       </c>
-      <c r="B13" s="248" t="s">
+      <c r="B13" s="252" t="s">
         <v>187</v>
       </c>
-      <c r="C13" s="247"/>
-      <c r="D13" s="247"/>
-      <c r="E13" s="247"/>
-      <c r="F13" s="247"/>
-      <c r="G13" s="174"/>
+      <c r="C13" s="249"/>
+      <c r="D13" s="249"/>
+      <c r="E13" s="249"/>
+      <c r="F13" s="249"/>
+      <c r="G13" s="176"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
@@ -13260,14 +13304,14 @@
       <c r="A14" s="148" t="s">
         <v>188</v>
       </c>
-      <c r="B14" s="248" t="s">
+      <c r="B14" s="252" t="s">
         <v>189</v>
       </c>
-      <c r="C14" s="247"/>
-      <c r="D14" s="247"/>
-      <c r="E14" s="247"/>
-      <c r="F14" s="247"/>
-      <c r="G14" s="174"/>
+      <c r="C14" s="249"/>
+      <c r="D14" s="249"/>
+      <c r="E14" s="249"/>
+      <c r="F14" s="249"/>
+      <c r="G14" s="176"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -13278,14 +13322,14 @@
       <c r="A15" s="148" t="s">
         <v>190</v>
       </c>
-      <c r="B15" s="249" t="s">
+      <c r="B15" s="250" t="s">
         <v>191</v>
       </c>
-      <c r="C15" s="250"/>
-      <c r="D15" s="250"/>
-      <c r="E15" s="250"/>
-      <c r="F15" s="250"/>
-      <c r="G15" s="195"/>
+      <c r="C15" s="251"/>
+      <c r="D15" s="251"/>
+      <c r="E15" s="251"/>
+      <c r="F15" s="251"/>
+      <c r="G15" s="216"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>

</xml_diff>